<commit_message>
Crunched pop growth data
</commit_message>
<xml_diff>
--- a/reg_housing_raw.xlsx
+++ b/reg_housing_raw.xlsx
@@ -1,68 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eclute\GitHub\regional-data-profile\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258D4BBC-342F-4A00-9E93-8061FB0F0698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="chart_1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="chart_2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="chart_3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="chart_4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="chart_1" sheetId="1" r:id="rId1"/>
+    <sheet name="chart_2" sheetId="2" r:id="rId2"/>
+    <sheet name="chart_3" sheetId="3" r:id="rId3"/>
+    <sheet name="chart_4" sheetId="4" r:id="rId4"/>
+    <sheet name="Housing" sheetId="5" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
   <si>
-    <t xml:space="preserve">year</t>
+    <t>year</t>
   </si>
   <si>
-    <t xml:space="preserve">King</t>
+    <t>King</t>
   </si>
   <si>
-    <t xml:space="preserve">Kitsap</t>
+    <t>Kitsap</t>
   </si>
   <si>
-    <t xml:space="preserve">Pierce</t>
+    <t>Pierce</t>
   </si>
   <si>
-    <t xml:space="preserve">Snohomish</t>
+    <t>Snohomish</t>
   </si>
   <si>
-    <t xml:space="preserve">source_info</t>
+    <t>source_info</t>
   </si>
   <si>
-    <t xml:space="preserve">OFM April 1 Housing Estimates. Data representing 2000 thru 2024. Calculated by Eric Clute.</t>
+    <t>geography</t>
   </si>
   <si>
-    <t xml:space="preserve">geography</t>
+    <t>sf</t>
   </si>
   <si>
-    <t xml:space="preserve">sf</t>
+    <t>mf</t>
   </si>
   <si>
-    <t xml:space="preserve">mf</t>
+    <t>mh</t>
   </si>
   <si>
-    <t xml:space="preserve">mh</t>
+    <t>total</t>
   </si>
   <si>
-    <t xml:space="preserve">total</t>
+    <t>Region</t>
   </si>
   <si>
-    <t xml:space="preserve">Region</t>
+    <t>OFM April 1 Housing Estimates. Data representing 2010 thru 2024. Calculated by Eric Clute.</t>
+  </si>
+  <si>
+    <t>Chart #1</t>
+  </si>
+  <si>
+    <t>Chart #2</t>
+  </si>
+  <si>
+    <t>Chart #3</t>
+  </si>
+  <si>
+    <t>Chart #4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -90,13 +118,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -378,14 +416,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,390 +442,394 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>2010</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>851261</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>107367</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>325375</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>286659</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>2011</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>857258</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>107364</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>327375</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>288520</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>2012</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>862221</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>107858</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>329157</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>290714</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>2013</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>870086</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>108449</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>331860</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>293600</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>2014</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>880304</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>109136</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>335161</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>297426</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>894045</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>109474</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>338304</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>300707</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>2016</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>907354</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>110385</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>341404</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>304394</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>2017</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>922163</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>111145</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>345681</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>307950</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>2018</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>937249</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>112344</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>349424</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>312718</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>2019</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>956082</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>113145</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>353085</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>316948</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>2020</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>969234</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>113248</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>359489</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>321523</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>2021</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>984458</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>114252</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>364156</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>326723</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>2022</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>1002063</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>115403</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>368424</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>331192</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>2023</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>1020458</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>116977</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>372102</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>336689</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>2024</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>1040144</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>118752</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>376621</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>341277</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="A1:F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2010</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>980233</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>515753</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>74676</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>1570662</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3">
         <v>1049316</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>638942</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>75236</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>1763494</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>2024</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4">
         <v>1076342</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>724544</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>75908</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>1876794</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,193 +846,790 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>2024</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1040144</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>118752</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>376621</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>341277</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>1876794</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>2010</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1570662</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>2011</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1580517</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>2012</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>1589950</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>2013</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>1603995</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>2014</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>1622027</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>1642530</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>2016</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>1663537</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>2017</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>1686939</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>2018</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>1711735</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>2019</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>1739260</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>2020</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>1763494</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>2021</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>1789589</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>2022</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>1817082</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>2023</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>1846226</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>2024</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>1876794</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1D7E18-8085-4B2B-BDA3-39E8D8D7F9A0}">
+  <dimension ref="A1:F57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2010</v>
+      </c>
+      <c r="B3">
+        <v>851261</v>
+      </c>
+      <c r="C3">
+        <v>107367</v>
+      </c>
+      <c r="D3">
+        <v>325375</v>
+      </c>
+      <c r="E3">
+        <v>286659</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4">
+        <v>857258</v>
+      </c>
+      <c r="C4">
+        <v>107364</v>
+      </c>
+      <c r="D4">
+        <v>327375</v>
+      </c>
+      <c r="E4">
+        <v>288520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2012</v>
+      </c>
+      <c r="B5">
+        <v>862221</v>
+      </c>
+      <c r="C5">
+        <v>107858</v>
+      </c>
+      <c r="D5">
+        <v>329157</v>
+      </c>
+      <c r="E5">
+        <v>290714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2013</v>
+      </c>
+      <c r="B6">
+        <v>870086</v>
+      </c>
+      <c r="C6">
+        <v>108449</v>
+      </c>
+      <c r="D6">
+        <v>331860</v>
+      </c>
+      <c r="E6">
+        <v>293600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7">
+        <v>880304</v>
+      </c>
+      <c r="C7">
+        <v>109136</v>
+      </c>
+      <c r="D7">
+        <v>335161</v>
+      </c>
+      <c r="E7">
+        <v>297426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2015</v>
+      </c>
+      <c r="B8">
+        <v>894045</v>
+      </c>
+      <c r="C8">
+        <v>109474</v>
+      </c>
+      <c r="D8">
+        <v>338304</v>
+      </c>
+      <c r="E8">
+        <v>300707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2016</v>
+      </c>
+      <c r="B9">
+        <v>907354</v>
+      </c>
+      <c r="C9">
+        <v>110385</v>
+      </c>
+      <c r="D9">
+        <v>341404</v>
+      </c>
+      <c r="E9">
+        <v>304394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2017</v>
+      </c>
+      <c r="B10">
+        <v>922163</v>
+      </c>
+      <c r="C10">
+        <v>111145</v>
+      </c>
+      <c r="D10">
+        <v>345681</v>
+      </c>
+      <c r="E10">
+        <v>307950</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2018</v>
+      </c>
+      <c r="B11">
+        <v>937249</v>
+      </c>
+      <c r="C11">
+        <v>112344</v>
+      </c>
+      <c r="D11">
+        <v>349424</v>
+      </c>
+      <c r="E11">
+        <v>312718</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2019</v>
+      </c>
+      <c r="B12">
+        <v>956082</v>
+      </c>
+      <c r="C12">
+        <v>113145</v>
+      </c>
+      <c r="D12">
+        <v>353085</v>
+      </c>
+      <c r="E12">
+        <v>316948</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2020</v>
+      </c>
+      <c r="B13">
+        <v>969234</v>
+      </c>
+      <c r="C13">
+        <v>113248</v>
+      </c>
+      <c r="D13">
+        <v>359489</v>
+      </c>
+      <c r="E13">
+        <v>321523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2021</v>
+      </c>
+      <c r="B14">
+        <v>984458</v>
+      </c>
+      <c r="C14">
+        <v>114252</v>
+      </c>
+      <c r="D14">
+        <v>364156</v>
+      </c>
+      <c r="E14">
+        <v>326723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2022</v>
+      </c>
+      <c r="B15">
+        <v>1002063</v>
+      </c>
+      <c r="C15">
+        <v>115403</v>
+      </c>
+      <c r="D15">
+        <v>368424</v>
+      </c>
+      <c r="E15">
+        <v>331192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2023</v>
+      </c>
+      <c r="B16">
+        <v>1020458</v>
+      </c>
+      <c r="C16">
+        <v>116977</v>
+      </c>
+      <c r="D16">
+        <v>372102</v>
+      </c>
+      <c r="E16">
+        <v>336689</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2024</v>
+      </c>
+      <c r="B17">
+        <v>1040144</v>
+      </c>
+      <c r="C17">
+        <v>118752</v>
+      </c>
+      <c r="D17">
+        <v>376621</v>
+      </c>
+      <c r="E17">
+        <v>341277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2010</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>980233</v>
+      </c>
+      <c r="D24">
+        <v>515753</v>
+      </c>
+      <c r="E24">
+        <v>74676</v>
+      </c>
+      <c r="F24">
+        <v>1570662</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2020</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>1049316</v>
+      </c>
+      <c r="D25">
+        <v>638942</v>
+      </c>
+      <c r="E25">
+        <v>75236</v>
+      </c>
+      <c r="F25">
+        <v>1763494</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2024</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>1076342</v>
+      </c>
+      <c r="D26">
+        <v>724544</v>
+      </c>
+      <c r="E26">
+        <v>75908</v>
+      </c>
+      <c r="F26">
+        <v>1876794</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2024</v>
+      </c>
+      <c r="B33">
+        <v>1040144</v>
+      </c>
+      <c r="C33">
+        <v>118752</v>
+      </c>
+      <c r="D33">
+        <v>376621</v>
+      </c>
+      <c r="E33">
+        <v>341277</v>
+      </c>
+      <c r="F33">
+        <v>1876794</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2010</v>
+      </c>
+      <c r="B40">
+        <v>1570662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>2011</v>
+      </c>
+      <c r="B41">
+        <v>1580517</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>2012</v>
+      </c>
+      <c r="B42">
+        <v>1589950</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2013</v>
+      </c>
+      <c r="B43">
+        <v>1603995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2014</v>
+      </c>
+      <c r="B44">
+        <v>1622027</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2015</v>
+      </c>
+      <c r="B45">
+        <v>1642530</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>2016</v>
+      </c>
+      <c r="B46">
+        <v>1663537</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>2017</v>
+      </c>
+      <c r="B47">
+        <v>1686939</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>2018</v>
+      </c>
+      <c r="B48">
+        <v>1711735</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2019</v>
+      </c>
+      <c r="B49">
+        <v>1739260</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>2020</v>
+      </c>
+      <c r="B50">
+        <v>1763494</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>2021</v>
+      </c>
+      <c r="B51">
+        <v>1789589</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>2022</v>
+      </c>
+      <c r="B52">
+        <v>1817082</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>2023</v>
+      </c>
+      <c r="B53">
+        <v>1846226</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>2024</v>
+      </c>
+      <c r="B54">
+        <v>1876794</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>